<commit_message>
Update Copy of room_design_abs_final.xlsx
</commit_message>
<xml_diff>
--- a/RoomAcoustics/modulo 2/1_room_design_absorption/Copy of room_design_abs_final.xlsx
+++ b/RoomAcoustics/modulo 2/1_room_design_absorption/Copy of room_design_abs_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i7\Documents\GitHub\MusicalAcousticsHWs\RoomAcoustics\modulo 2\1_room_design_absorption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F675CAE3-183A-49A3-94B9-6B9545ABB04E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A878D536-86C2-4D2C-B555-6621E6FFD7DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="761" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="761" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -1237,6 +1237,12 @@
     <xf numFmtId="0" fontId="19" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1249,16 +1255,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1282,10 +1279,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1294,22 +1303,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1318,34 +1315,37 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -15766,7 +15766,7 @@
               <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Angsana New" panose="020B0502040204020203" pitchFamily="18" charset="-34"/>
             </a:rPr>
-            <a:t> averaged is actually varies very little between first three cases. When we change material (case C) instead deviation values display a considerable variation. </a:t>
+            <a:t> averaged  actually varies very little between first three cases. When we change material (case C) instead deviation values display a considerable variation. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -16076,14 +16076,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="85"/>
+      <c r="E1" s="87"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="2">
@@ -16097,20 +16097,20 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="90" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="87"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -16246,14 +16246,14 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85" t="s">
+      <c r="C14" s="87"/>
+      <c r="D14" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="85"/>
+      <c r="E14" s="87"/>
     </row>
     <row r="15" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
@@ -16388,7 +16388,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
@@ -16417,18 +16417,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="N1" s="93" t="s">
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="N1" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -16461,10 +16461,10 @@
       <c r="J2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="98" t="s">
+      <c r="N2" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="99"/>
+      <c r="O2" s="98"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
@@ -16502,11 +16502,11 @@
       <c r="J4" s="9">
         <v>0.28000000000000003</v>
       </c>
-      <c r="N4" s="94">
+      <c r="N4" s="93">
         <f>1/(surface_A)*(C4*area_S1+D4*area_S2+E4*area_S3+F4*area_S4+G4*area_S5_1+H4*area_S5_2+I4*area_S6+J4*area_S7)</f>
         <v>0.14322978529008681</v>
       </c>
-      <c r="O4" s="95"/>
+      <c r="O4" s="94"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
@@ -16540,11 +16540,11 @@
       <c r="J5" s="9">
         <v>0.25</v>
       </c>
-      <c r="N5" s="94">
+      <c r="N5" s="93">
         <f t="shared" ref="N5:N9" si="0">1/(surface_A)*(C5*area_S1+D5*area_S2+E5*area_S3+F5*area_S4+G5*area_S5_1+H5*area_S5_2+I5*area_S6+J5*area_S7)</f>
         <v>0.10523069894929193</v>
       </c>
-      <c r="O5" s="95"/>
+      <c r="O5" s="94"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
@@ -16578,11 +16578,11 @@
       <c r="J6" s="9">
         <v>0.18</v>
       </c>
-      <c r="N6" s="94">
+      <c r="N6" s="93">
         <f t="shared" si="0"/>
         <v>9.174280493375972E-2</v>
       </c>
-      <c r="O6" s="95"/>
+      <c r="O6" s="94"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
@@ -16616,11 +16616,11 @@
       <c r="J7" s="9">
         <v>0.12</v>
       </c>
-      <c r="N7" s="94">
+      <c r="N7" s="93">
         <f t="shared" si="0"/>
         <v>6.7512562814070379E-2</v>
       </c>
-      <c r="O7" s="95"/>
+      <c r="O7" s="94"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
@@ -16654,11 +16654,11 @@
       <c r="J8" s="9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N8" s="94">
+      <c r="N8" s="93">
         <f t="shared" si="0"/>
         <v>6.1685701233439943E-2</v>
       </c>
-      <c r="O8" s="95"/>
+      <c r="O8" s="94"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
@@ -16692,36 +16692,36 @@
       <c r="J9" s="9">
         <v>0.04</v>
       </c>
-      <c r="N9" s="94">
+      <c r="N9" s="93">
         <f t="shared" si="0"/>
         <v>6.1831886706258575E-2</v>
       </c>
-      <c r="O9" s="95"/>
+      <c r="O9" s="94"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="100"/>
-      <c r="I11" s="89" t="s">
+      <c r="B11" s="91"/>
+      <c r="I11" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="89"/>
-      <c r="M11" s="93" t="s">
+      <c r="J11" s="99"/>
+      <c r="M11" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="N11" s="93"/>
-      <c r="O11" s="93"/>
-      <c r="P11" s="93"/>
+      <c r="N11" s="92"/>
+      <c r="O11" s="92"/>
+      <c r="P11" s="92"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="100"/>
+      <c r="B12" s="91"/>
       <c r="I12" s="12" t="s">
         <v>17</v>
       </c>
@@ -16732,23 +16732,23 @@
       <c r="M12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="96" t="s">
+      <c r="N12" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="O12" s="97"/>
+      <c r="O12" s="96"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="100"/>
+      <c r="B13" s="91"/>
       <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="100"/>
+      <c r="B14" s="91"/>
       <c r="I14" s="12">
         <v>125</v>
       </c>
@@ -16759,17 +16759,17 @@
       <c r="M14" s="11">
         <v>125</v>
       </c>
-      <c r="N14" s="91">
+      <c r="N14" s="101">
         <f t="shared" ref="N14:N19" si="3">(N4*surface_A)/(1-N4)</f>
         <v>36.594409401376723</v>
       </c>
-      <c r="O14" s="92"/>
+      <c r="O14" s="102"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="100"/>
+      <c r="B15" s="91"/>
       <c r="I15" s="12">
         <v>250</v>
       </c>
@@ -16780,17 +16780,17 @@
       <c r="M15" s="11">
         <v>250</v>
       </c>
-      <c r="N15" s="91">
+      <c r="N15" s="101">
         <f t="shared" si="3"/>
         <v>25.744066065912751</v>
       </c>
-      <c r="O15" s="92"/>
+      <c r="O15" s="102"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="100"/>
+      <c r="B16" s="91"/>
       <c r="I16" s="12">
         <v>500</v>
       </c>
@@ -16801,17 +16801,17 @@
       <c r="M16" s="11">
         <v>500</v>
       </c>
-      <c r="N16" s="91">
+      <c r="N16" s="101">
         <f t="shared" si="3"/>
         <v>22.111027701283842</v>
       </c>
-      <c r="O16" s="92"/>
+      <c r="O16" s="102"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="100" t="s">
+      <c r="A17" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="100"/>
+      <c r="B17" s="91"/>
       <c r="I17" s="12">
         <v>1000</v>
       </c>
@@ -16822,11 +16822,11 @@
       <c r="M17" s="11">
         <v>1000</v>
       </c>
-      <c r="N17" s="91">
+      <c r="N17" s="101">
         <f t="shared" si="3"/>
         <v>15.848470886212384</v>
       </c>
-      <c r="O17" s="92"/>
+      <c r="O17" s="102"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I18" s="12">
@@ -16839,11 +16839,11 @@
       <c r="M18" s="11">
         <v>2000</v>
       </c>
-      <c r="N18" s="91">
+      <c r="N18" s="101">
         <f t="shared" si="3"/>
         <v>14.390700448399931</v>
       </c>
-      <c r="O18" s="92"/>
+      <c r="O18" s="102"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F19" s="13"/>
@@ -16857,25 +16857,25 @@
       <c r="M19" s="11">
         <v>4000</v>
       </c>
-      <c r="N19" s="91">
+      <c r="N19" s="101">
         <f t="shared" si="3"/>
         <v>14.427051834538505</v>
       </c>
-      <c r="O19" s="92"/>
+      <c r="O19" s="102"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C21" s="89" t="s">
+      <c r="C21" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="90"/>
-      <c r="E21" s="89" t="s">
+      <c r="D21" s="100"/>
+      <c r="E21" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="90"/>
-      <c r="I21" s="89" t="s">
+      <c r="F21" s="100"/>
+      <c r="I21" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="89"/>
+      <c r="J21" s="99"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
@@ -17023,23 +17023,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="C21:D21"/>
@@ -17051,6 +17034,23 @@
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="N17:O17"/>
     <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17076,18 +17076,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="N1" s="93" t="s">
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="N1" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -17120,10 +17120,10 @@
       <c r="J2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="98" t="s">
+      <c r="N2" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="99"/>
+      <c r="O2" s="98"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
@@ -17161,11 +17161,11 @@
       <c r="J4" s="9">
         <v>0.28000000000000003</v>
       </c>
-      <c r="N4" s="94">
+      <c r="N4" s="93">
         <f t="shared" ref="N4:N9" si="0">1/(surface_B1)*(C4*area_S1_B1+D4*area_S2_B1+E4*area_S3_B1+F4*area_S4_B1+G4*area_S5_B1_1+H4*area_S5_B1_2+I4*area_S6_B1+J4*area_S7_B1)</f>
         <v>0.14411021814006889</v>
       </c>
-      <c r="O4" s="95"/>
+      <c r="O4" s="94"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
@@ -17199,11 +17199,11 @@
       <c r="J5" s="9">
         <v>0.25</v>
       </c>
-      <c r="N5" s="94">
+      <c r="N5" s="93">
         <f t="shared" si="0"/>
         <v>0.10610792192881746</v>
       </c>
-      <c r="O5" s="95"/>
+      <c r="O5" s="94"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
@@ -17237,11 +17237,11 @@
       <c r="J6" s="9">
         <v>0.18</v>
       </c>
-      <c r="N6" s="94">
+      <c r="N6" s="93">
         <f t="shared" si="0"/>
         <v>9.2353616532721006E-2</v>
       </c>
-      <c r="O6" s="95"/>
+      <c r="O6" s="94"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
@@ -17275,11 +17275,11 @@
       <c r="J7" s="9">
         <v>0.12</v>
       </c>
-      <c r="N7" s="94">
+      <c r="N7" s="93">
         <f t="shared" si="0"/>
         <v>6.7967853042479931E-2</v>
       </c>
-      <c r="O7" s="95"/>
+      <c r="O7" s="94"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
@@ -17313,11 +17313,11 @@
       <c r="J8" s="9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N8" s="94">
+      <c r="N8" s="93">
         <f t="shared" si="0"/>
         <v>6.1980482204362801E-2</v>
       </c>
-      <c r="O8" s="95"/>
+      <c r="O8" s="94"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
@@ -17351,36 +17351,36 @@
       <c r="J9" s="9">
         <v>0.04</v>
       </c>
-      <c r="N9" s="94">
+      <c r="N9" s="93">
         <f t="shared" si="0"/>
         <v>6.1923076923076942E-2</v>
       </c>
-      <c r="O9" s="95"/>
+      <c r="O9" s="94"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="100"/>
-      <c r="I11" s="89" t="s">
+      <c r="B11" s="91"/>
+      <c r="I11" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="89"/>
-      <c r="M11" s="93" t="s">
+      <c r="J11" s="99"/>
+      <c r="M11" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="N11" s="93"/>
-      <c r="O11" s="93"/>
-      <c r="P11" s="93"/>
+      <c r="N11" s="92"/>
+      <c r="O11" s="92"/>
+      <c r="P11" s="92"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="100"/>
+      <c r="B12" s="91"/>
       <c r="I12" s="12" t="s">
         <v>17</v>
       </c>
@@ -17391,23 +17391,23 @@
       <c r="M12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="96" t="s">
+      <c r="N12" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="O12" s="97"/>
+      <c r="O12" s="96"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="100"/>
+      <c r="B13" s="91"/>
       <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="100"/>
+      <c r="B14" s="91"/>
       <c r="I14" s="12">
         <v>125</v>
       </c>
@@ -17418,17 +17418,17 @@
       <c r="M14" s="11">
         <v>125</v>
       </c>
-      <c r="N14" s="91">
+      <c r="N14" s="101">
         <f t="shared" ref="N14:N19" si="3">(N4*surface_B1)/(1-N4)</f>
         <v>23.464703546708158</v>
       </c>
-      <c r="O14" s="92"/>
+      <c r="O14" s="102"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="100"/>
+      <c r="B15" s="91"/>
       <c r="I15" s="12">
         <v>250</v>
       </c>
@@ -17439,17 +17439,17 @@
       <c r="M15" s="11">
         <v>250</v>
       </c>
-      <c r="N15" s="91">
+      <c r="N15" s="101">
         <f t="shared" si="3"/>
         <v>16.542489146908476</v>
       </c>
-      <c r="O15" s="92"/>
+      <c r="O15" s="102"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="100"/>
+      <c r="B16" s="91"/>
       <c r="I16" s="12">
         <v>500</v>
       </c>
@@ -17460,17 +17460,17 @@
       <c r="M16" s="11">
         <v>500</v>
       </c>
-      <c r="N16" s="91">
+      <c r="N16" s="101">
         <f t="shared" si="3"/>
         <v>14.179971665654724</v>
       </c>
-      <c r="O16" s="92"/>
+      <c r="O16" s="102"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="100" t="s">
+      <c r="A17" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="100"/>
+      <c r="B17" s="91"/>
       <c r="I17" s="12">
         <v>1000</v>
       </c>
@@ -17481,11 +17481,11 @@
       <c r="M17" s="11">
         <v>1000</v>
       </c>
-      <c r="N17" s="91">
+      <c r="N17" s="101">
         <f t="shared" si="3"/>
         <v>10.162739591032276</v>
       </c>
-      <c r="O17" s="92"/>
+      <c r="O17" s="102"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I18" s="12">
@@ -17498,11 +17498,11 @@
       <c r="M18" s="11">
         <v>2000</v>
       </c>
-      <c r="N18" s="91">
+      <c r="N18" s="101">
         <f t="shared" si="3"/>
         <v>9.2083371786319699</v>
       </c>
-      <c r="O18" s="92"/>
+      <c r="O18" s="102"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F19" s="13"/>
@@ -17516,25 +17516,25 @@
       <c r="M19" s="11">
         <v>4000</v>
       </c>
-      <c r="N19" s="91">
+      <c r="N19" s="101">
         <f t="shared" si="3"/>
         <v>9.1992455924559273</v>
       </c>
-      <c r="O19" s="92"/>
+      <c r="O19" s="102"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C21" s="89" t="s">
+      <c r="C21" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="90"/>
-      <c r="E21" s="89" t="s">
+      <c r="D21" s="100"/>
+      <c r="E21" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="90"/>
-      <c r="I21" s="89" t="s">
+      <c r="F21" s="100"/>
+      <c r="I21" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="89"/>
+      <c r="J21" s="99"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
@@ -17682,12 +17682,15 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="N7:O7"/>
@@ -17701,15 +17704,12 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="N14:O14"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -17734,18 +17734,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="N1" s="93" t="s">
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="N1" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -17778,10 +17778,10 @@
       <c r="J2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="98" t="s">
+      <c r="N2" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="99"/>
+      <c r="O2" s="98"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
@@ -17819,11 +17819,11 @@
       <c r="J4" s="9">
         <v>0.28000000000000003</v>
       </c>
-      <c r="N4" s="94">
+      <c r="N4" s="93">
         <f t="shared" ref="N4:N9" si="0">1/(surface_B2)*(C4*area_S1_B2+D4*area_S2_B2+E4*area_S3_B2+F4*area_S4_B2+G4*area_S5_B2_1+H4*area_S5_B2_2+I4*area_S6_B2+J4*area_S7_B2)</f>
         <v>0.14211076923076923</v>
       </c>
-      <c r="O4" s="95"/>
+      <c r="O4" s="94"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
@@ -17857,11 +17857,11 @@
       <c r="J5" s="9">
         <v>0.25</v>
       </c>
-      <c r="N5" s="94">
+      <c r="N5" s="93">
         <f t="shared" si="0"/>
         <v>0.10518769230769233</v>
       </c>
-      <c r="O5" s="95"/>
+      <c r="O5" s="94"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
@@ -17895,11 +17895,11 @@
       <c r="J6" s="9">
         <v>0.18</v>
       </c>
-      <c r="N6" s="94">
+      <c r="N6" s="93">
         <f t="shared" si="0"/>
         <v>8.8841538461538472E-2</v>
       </c>
-      <c r="O6" s="95"/>
+      <c r="O6" s="94"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
@@ -17933,11 +17933,11 @@
       <c r="J7" s="9">
         <v>0.12</v>
       </c>
-      <c r="N7" s="94">
+      <c r="N7" s="93">
         <f t="shared" si="0"/>
         <v>6.7490769230769229E-2</v>
       </c>
-      <c r="O7" s="95"/>
+      <c r="O7" s="94"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
@@ -17971,11 +17971,11 @@
       <c r="J8" s="9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N8" s="94">
+      <c r="N8" s="93">
         <f t="shared" si="0"/>
         <v>6.3344615384615388E-2</v>
       </c>
-      <c r="O8" s="95"/>
+      <c r="O8" s="94"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
@@ -18009,36 +18009,36 @@
       <c r="J9" s="9">
         <v>0.04</v>
       </c>
-      <c r="N9" s="94">
+      <c r="N9" s="93">
         <f t="shared" si="0"/>
         <v>5.7200000000000001E-2</v>
       </c>
-      <c r="O9" s="95"/>
+      <c r="O9" s="94"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="100"/>
-      <c r="I11" s="89" t="s">
+      <c r="B11" s="91"/>
+      <c r="I11" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="89"/>
-      <c r="M11" s="93" t="s">
+      <c r="J11" s="99"/>
+      <c r="M11" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="N11" s="93"/>
-      <c r="O11" s="93"/>
-      <c r="P11" s="93"/>
+      <c r="N11" s="92"/>
+      <c r="O11" s="92"/>
+      <c r="P11" s="92"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="100"/>
+      <c r="B12" s="91"/>
       <c r="I12" s="12" t="s">
         <v>17</v>
       </c>
@@ -18049,23 +18049,23 @@
       <c r="M12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="96" t="s">
+      <c r="N12" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="O12" s="97"/>
+      <c r="O12" s="96"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="100"/>
+      <c r="B13" s="91"/>
       <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="100"/>
+      <c r="B14" s="91"/>
       <c r="I14" s="12">
         <v>125</v>
       </c>
@@ -18076,17 +18076,17 @@
       <c r="M14" s="11">
         <v>125</v>
       </c>
-      <c r="N14" s="91">
+      <c r="N14" s="101">
         <f t="shared" ref="N14:N19" si="3">(N4*surface_B2)/(1-N4)</f>
         <v>21.534714899538759</v>
       </c>
-      <c r="O14" s="92"/>
+      <c r="O14" s="102"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="100"/>
+      <c r="B15" s="91"/>
       <c r="I15" s="12">
         <v>250</v>
       </c>
@@ -18097,17 +18097,17 @@
       <c r="M15" s="11">
         <v>250</v>
       </c>
-      <c r="N15" s="91">
+      <c r="N15" s="101">
         <f t="shared" si="3"/>
         <v>15.281864009298042</v>
       </c>
-      <c r="O15" s="92"/>
+      <c r="O15" s="102"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="100"/>
+      <c r="B16" s="91"/>
       <c r="I16" s="12">
         <v>500</v>
       </c>
@@ -18118,17 +18118,17 @@
       <c r="M16" s="11">
         <v>500</v>
       </c>
-      <c r="N16" s="91">
+      <c r="N16" s="101">
         <f t="shared" si="3"/>
         <v>12.675511985587242</v>
       </c>
-      <c r="O16" s="92"/>
+      <c r="O16" s="102"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="100" t="s">
+      <c r="A17" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="100"/>
+      <c r="B17" s="91"/>
       <c r="I17" s="12">
         <v>1000</v>
       </c>
@@ -18139,11 +18139,11 @@
       <c r="M17" s="11">
         <v>1000</v>
       </c>
-      <c r="N17" s="91">
+      <c r="N17" s="101">
         <f t="shared" si="3"/>
         <v>9.4088076669894782</v>
       </c>
-      <c r="O17" s="92"/>
+      <c r="O17" s="102"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I18" s="12">
@@ -18156,11 +18156,11 @@
       <c r="M18" s="11">
         <v>2000</v>
       </c>
-      <c r="N18" s="91">
+      <c r="N18" s="101">
         <f t="shared" si="3"/>
         <v>8.7917073186756145</v>
       </c>
-      <c r="O18" s="92"/>
+      <c r="O18" s="102"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F19" s="13"/>
@@ -18174,25 +18174,25 @@
       <c r="M19" s="11">
         <v>4000</v>
       </c>
-      <c r="N19" s="91">
+      <c r="N19" s="101">
         <f t="shared" si="3"/>
         <v>7.8871446754348753</v>
       </c>
-      <c r="O19" s="92"/>
+      <c r="O19" s="102"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C21" s="89" t="s">
+      <c r="C21" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="90"/>
-      <c r="E21" s="89" t="s">
+      <c r="D21" s="100"/>
+      <c r="E21" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="90"/>
-      <c r="I21" s="89" t="s">
+      <c r="F21" s="100"/>
+      <c r="I21" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="89"/>
+      <c r="J21" s="99"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
@@ -18340,12 +18340,15 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="N7:O7"/>
@@ -18359,15 +18362,12 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="N14:O14"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18381,7 +18381,7 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4:D9"/>
     </sheetView>
   </sheetViews>
@@ -18392,18 +18392,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="N1" s="93" t="s">
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="N1" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -18439,10 +18439,10 @@
       <c r="K2" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="98" t="s">
+      <c r="N2" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="99"/>
+      <c r="O2" s="98"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
@@ -18483,11 +18483,11 @@
       <c r="K4" s="9">
         <v>0.3</v>
       </c>
-      <c r="N4" s="94">
+      <c r="N4" s="93">
         <f t="shared" ref="N4:N9" si="0">1/(surface_A)*(0.4*C4*area_S1+D4*area_S2+E4*area_S3+F4*area_S4+G4*area_S5_1+H4*area_S5_2+I4*area_S6+J4*area_S7 + 0.6*K4*area_S1)</f>
         <v>0.19950890817724987</v>
       </c>
-      <c r="O4" s="95"/>
+      <c r="O4" s="94"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
@@ -18524,11 +18524,11 @@
       <c r="K5" s="9">
         <v>0.41</v>
       </c>
-      <c r="N5" s="94">
+      <c r="N5" s="93">
         <f t="shared" si="0"/>
         <v>0.22120146185472822</v>
       </c>
-      <c r="O5" s="95"/>
+      <c r="O5" s="94"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
@@ -18565,11 +18565,11 @@
       <c r="K6" s="9">
         <v>0.49</v>
       </c>
-      <c r="N6" s="94">
+      <c r="N6" s="93">
         <f t="shared" si="0"/>
         <v>0.2563302878026496</v>
       </c>
-      <c r="O6" s="95"/>
+      <c r="O6" s="94"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
@@ -18606,11 +18606,11 @@
       <c r="K7" s="9">
         <v>0.84</v>
       </c>
-      <c r="N7" s="94">
+      <c r="N7" s="93">
         <f t="shared" si="0"/>
         <v>0.28933576975788033</v>
       </c>
-      <c r="O7" s="95"/>
+      <c r="O7" s="94"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
@@ -18647,11 +18647,11 @@
       <c r="K8" s="9">
         <v>0.87</v>
       </c>
-      <c r="N8" s="94">
+      <c r="N8" s="93">
         <f t="shared" si="0"/>
         <v>0.293772498857926</v>
       </c>
-      <c r="O8" s="95"/>
+      <c r="O8" s="94"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
@@ -18688,36 +18688,36 @@
       <c r="K9" s="9">
         <v>0.84</v>
       </c>
-      <c r="N9" s="94">
+      <c r="N9" s="93">
         <f t="shared" si="0"/>
         <v>0.28408679762448608</v>
       </c>
-      <c r="O9" s="95"/>
+      <c r="O9" s="94"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="100"/>
-      <c r="I11" s="89" t="s">
+      <c r="B11" s="91"/>
+      <c r="I11" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="89"/>
-      <c r="M11" s="93" t="s">
+      <c r="J11" s="99"/>
+      <c r="M11" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="N11" s="93"/>
-      <c r="O11" s="93"/>
-      <c r="P11" s="93"/>
+      <c r="N11" s="92"/>
+      <c r="O11" s="92"/>
+      <c r="P11" s="92"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="100"/>
+      <c r="B12" s="91"/>
       <c r="I12" s="12" t="s">
         <v>17</v>
       </c>
@@ -18728,23 +18728,23 @@
       <c r="M12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="96" t="s">
+      <c r="N12" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="O12" s="97"/>
+      <c r="O12" s="96"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="100"/>
+      <c r="B13" s="91"/>
       <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="100"/>
+      <c r="B14" s="91"/>
       <c r="I14" s="12">
         <v>125</v>
       </c>
@@ -18755,17 +18755,17 @@
       <c r="M14" s="11">
         <v>125</v>
       </c>
-      <c r="N14" s="91">
+      <c r="N14" s="101">
         <f t="shared" ref="N14:N19" si="3">(N4*surface_A)/(1-N4)</f>
         <v>54.557134296842662</v>
       </c>
-      <c r="O14" s="92"/>
+      <c r="O14" s="102"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="100"/>
+      <c r="B15" s="91"/>
       <c r="I15" s="12">
         <v>250</v>
       </c>
@@ -18776,17 +18776,17 @@
       <c r="M15" s="11">
         <v>250</v>
       </c>
-      <c r="N15" s="91">
+      <c r="N15" s="101">
         <f t="shared" si="3"/>
         <v>62.173973920541535</v>
       </c>
-      <c r="O15" s="92"/>
+      <c r="O15" s="102"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="100"/>
+      <c r="B16" s="91"/>
       <c r="I16" s="12">
         <v>500</v>
       </c>
@@ -18797,17 +18797,17 @@
       <c r="M16" s="11">
         <v>500</v>
       </c>
-      <c r="N16" s="91">
+      <c r="N16" s="101">
         <f t="shared" si="3"/>
         <v>75.451102928755148</v>
       </c>
-      <c r="O16" s="92"/>
+      <c r="O16" s="102"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="100" t="s">
+      <c r="A17" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="100"/>
+      <c r="B17" s="91"/>
       <c r="I17" s="12">
         <v>1000</v>
       </c>
@@ -18818,11 +18818,11 @@
       <c r="M17" s="11">
         <v>1000</v>
       </c>
-      <c r="N17" s="91">
+      <c r="N17" s="101">
         <f t="shared" si="3"/>
         <v>89.121693909403433</v>
       </c>
-      <c r="O17" s="92"/>
+      <c r="O17" s="102"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I18" s="12">
@@ -18835,17 +18835,17 @@
       <c r="M18" s="11">
         <v>2000</v>
       </c>
-      <c r="N18" s="91">
+      <c r="N18" s="101">
         <f t="shared" si="3"/>
         <v>91.056776882812429</v>
       </c>
-      <c r="O18" s="92"/>
+      <c r="O18" s="102"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="103"/>
       <c r="F19" s="13"/>
       <c r="I19" s="12">
         <v>4000</v>
@@ -18857,25 +18857,25 @@
       <c r="M19" s="11">
         <v>4000</v>
       </c>
-      <c r="N19" s="91">
+      <c r="N19" s="101">
         <f t="shared" si="3"/>
         <v>86.863323366093766</v>
       </c>
-      <c r="O19" s="92"/>
+      <c r="O19" s="102"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C21" s="89" t="s">
+      <c r="C21" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="90"/>
-      <c r="E21" s="89" t="s">
+      <c r="D21" s="100"/>
+      <c r="E21" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="90"/>
-      <c r="I21" s="89" t="s">
+      <c r="F21" s="100"/>
+      <c r="I21" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="89"/>
+      <c r="J21" s="99"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
@@ -19023,12 +19023,16 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="N7:O7"/>
@@ -19042,16 +19046,12 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19076,22 +19076,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="121" t="s">
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="104" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="121"/>
-      <c r="N1" s="93" t="s">
+      <c r="H1" s="104"/>
+      <c r="N1" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -19127,10 +19127,10 @@
       <c r="K2" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="98" t="s">
+      <c r="N2" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="99"/>
+      <c r="O2" s="98"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
@@ -19171,11 +19171,11 @@
       <c r="K4" s="9">
         <v>0.3</v>
       </c>
-      <c r="N4" s="94">
+      <c r="N4" s="93">
         <f t="shared" ref="N4:N9" si="0">1/(surface_B1)*(0.4*C4*area_S1_B1+D4*area_S2_B1+E4*area_S3_B1+F4*area_S4_B1+G4*area_S5_B1_1+H4*area_S5_B1_2+I4*area_S6_B1+J4*area_S7_B1+0.6*K4*area_S1_B1)</f>
         <v>0.18063145809414469</v>
       </c>
-      <c r="O4" s="95"/>
+      <c r="O4" s="94"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
@@ -19212,11 +19212,11 @@
       <c r="K5" s="9">
         <v>0.41</v>
       </c>
-      <c r="N5" s="94">
+      <c r="N5" s="93">
         <f t="shared" si="0"/>
         <v>0.27305396096440876</v>
       </c>
-      <c r="O5" s="95"/>
+      <c r="O5" s="94"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
@@ -19253,11 +19253,11 @@
       <c r="K6" s="9">
         <v>0.49</v>
       </c>
-      <c r="N6" s="94">
+      <c r="N6" s="93">
         <f t="shared" si="0"/>
         <v>0.44091963260619982</v>
       </c>
-      <c r="O6" s="95"/>
+      <c r="O6" s="94"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
@@ -19294,11 +19294,11 @@
       <c r="K7" s="9">
         <v>0.84</v>
       </c>
-      <c r="N7" s="94">
+      <c r="N7" s="93">
         <f t="shared" si="0"/>
         <v>0.54718484500574061</v>
       </c>
-      <c r="O7" s="95"/>
+      <c r="O7" s="94"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
@@ -19335,11 +19335,11 @@
       <c r="K8" s="9">
         <v>0.87</v>
       </c>
-      <c r="N8" s="94">
+      <c r="N8" s="93">
         <f t="shared" si="0"/>
         <v>0.5401308840413318</v>
       </c>
-      <c r="O8" s="95"/>
+      <c r="O8" s="94"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
@@ -19376,36 +19376,36 @@
       <c r="K9" s="9">
         <v>0.84</v>
       </c>
-      <c r="N9" s="94">
+      <c r="N9" s="93">
         <f t="shared" si="0"/>
         <v>0.53591044776119412</v>
       </c>
-      <c r="O9" s="95"/>
+      <c r="O9" s="94"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="100"/>
-      <c r="I11" s="89" t="s">
+      <c r="B11" s="91"/>
+      <c r="I11" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="89"/>
-      <c r="M11" s="93" t="s">
+      <c r="J11" s="99"/>
+      <c r="M11" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="N11" s="93"/>
-      <c r="O11" s="93"/>
-      <c r="P11" s="93"/>
+      <c r="N11" s="92"/>
+      <c r="O11" s="92"/>
+      <c r="P11" s="92"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="100"/>
+      <c r="B12" s="91"/>
       <c r="I12" s="12" t="s">
         <v>17</v>
       </c>
@@ -19416,23 +19416,23 @@
       <c r="M12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="96" t="s">
+      <c r="N12" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="O12" s="97"/>
+      <c r="O12" s="96"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="100"/>
+      <c r="B13" s="91"/>
       <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="100"/>
+      <c r="B14" s="91"/>
       <c r="I14" s="12">
         <v>125</v>
       </c>
@@ -19443,17 +19443,17 @@
       <c r="M14" s="11">
         <v>125</v>
       </c>
-      <c r="N14" s="91">
+      <c r="N14" s="101">
         <f t="shared" ref="N14:N19" si="3">(N4*surface_B1)/(1-N4)</f>
         <v>30.722194851962396</v>
       </c>
-      <c r="O14" s="92"/>
+      <c r="O14" s="102"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="100"/>
+      <c r="B15" s="91"/>
       <c r="I15" s="12">
         <v>250</v>
       </c>
@@ -19464,17 +19464,17 @@
       <c r="M15" s="11">
         <v>250</v>
       </c>
-      <c r="N15" s="91">
+      <c r="N15" s="101">
         <f t="shared" si="3"/>
         <v>52.346113681949554</v>
       </c>
-      <c r="O15" s="92"/>
+      <c r="O15" s="102"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="100"/>
+      <c r="B16" s="91"/>
       <c r="I16" s="12">
         <v>500</v>
       </c>
@@ -19485,17 +19485,17 @@
       <c r="M16" s="11">
         <v>500</v>
       </c>
-      <c r="N16" s="91">
+      <c r="N16" s="101">
         <f t="shared" si="3"/>
         <v>109.9064885544779</v>
       </c>
-      <c r="O16" s="92"/>
+      <c r="O16" s="102"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="100" t="s">
+      <c r="A17" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="100"/>
+      <c r="B17" s="91"/>
       <c r="I17" s="12">
         <v>1000</v>
       </c>
@@ -19506,11 +19506,11 @@
       <c r="M17" s="11">
         <v>1000</v>
       </c>
-      <c r="N17" s="91">
+      <c r="N17" s="101">
         <f t="shared" si="3"/>
         <v>168.40355089477237</v>
       </c>
-      <c r="O17" s="92"/>
+      <c r="O17" s="102"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I18" s="12">
@@ -19523,11 +19523,11 @@
       <c r="M18" s="11">
         <v>2000</v>
       </c>
-      <c r="N18" s="91">
+      <c r="N18" s="101">
         <f t="shared" si="3"/>
         <v>163.68274665082163</v>
       </c>
-      <c r="O18" s="92"/>
+      <c r="O18" s="102"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F19" s="13"/>
@@ -19541,25 +19541,25 @@
       <c r="M19" s="11">
         <v>4000</v>
       </c>
-      <c r="N19" s="91">
+      <c r="N19" s="101">
         <f t="shared" si="3"/>
         <v>160.92687206535027</v>
       </c>
-      <c r="O19" s="92"/>
+      <c r="O19" s="102"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C21" s="89" t="s">
+      <c r="C21" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="90"/>
-      <c r="E21" s="89" t="s">
+      <c r="D21" s="100"/>
+      <c r="E21" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="90"/>
-      <c r="I21" s="89" t="s">
+      <c r="F21" s="100"/>
+      <c r="I21" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="89"/>
+      <c r="J21" s="99"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
@@ -19707,13 +19707,15 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="N7:O7"/>
@@ -19727,15 +19729,13 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="N14:O14"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19760,18 +19760,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="N1" s="93" t="s">
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="N1" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -19807,10 +19807,10 @@
       <c r="K2" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="98" t="s">
+      <c r="N2" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="99"/>
+      <c r="O2" s="98"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
@@ -19851,11 +19851,11 @@
       <c r="K4" s="9">
         <v>0.3</v>
       </c>
-      <c r="N4" s="94">
+      <c r="N4" s="93">
         <f t="shared" ref="N4:N9" si="0">1/(surface_B2)*(0.4*C4*area_S1_B2+D4*area_S2_B2+E4*area_S3_B2+F4*area_S4_B2+G4*area_S5_B2_1+H4*area_S5_B2_2+I4*area_S6_B2+J4*area_S7_B2 + K4*0.6*area_S1_B2)</f>
         <v>0.19182153846153846</v>
       </c>
-      <c r="O4" s="95"/>
+      <c r="O4" s="94"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
@@ -19892,11 +19892,11 @@
       <c r="K5" s="9">
         <v>0.41</v>
       </c>
-      <c r="N5" s="94">
+      <c r="N5" s="93">
         <f t="shared" si="0"/>
         <v>0.26621846153846151</v>
       </c>
-      <c r="O5" s="95"/>
+      <c r="O5" s="94"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
@@ -19933,11 +19933,11 @@
       <c r="K6" s="9">
         <v>0.49</v>
       </c>
-      <c r="N6" s="94">
+      <c r="N6" s="93">
         <f t="shared" si="0"/>
         <v>0.38865538461538468</v>
       </c>
-      <c r="O6" s="95"/>
+      <c r="O6" s="94"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
@@ -19974,11 +19974,11 @@
       <c r="K7" s="9">
         <v>0.84</v>
       </c>
-      <c r="N7" s="94">
+      <c r="N7" s="93">
         <f t="shared" si="0"/>
         <v>0.43475230769230772</v>
       </c>
-      <c r="O7" s="95"/>
+      <c r="O7" s="94"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
@@ -20015,11 +20015,11 @@
       <c r="K8" s="9">
         <v>0.87</v>
       </c>
-      <c r="N8" s="94">
+      <c r="N8" s="93">
         <f t="shared" si="0"/>
         <v>0.43422307692307704</v>
       </c>
-      <c r="O8" s="95"/>
+      <c r="O8" s="94"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
@@ -20056,36 +20056,36 @@
       <c r="K9" s="9">
         <v>0.84</v>
       </c>
-      <c r="N9" s="94">
+      <c r="N9" s="93">
         <f t="shared" si="0"/>
         <v>0.42225692307692314</v>
       </c>
-      <c r="O9" s="95"/>
+      <c r="O9" s="94"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="100"/>
-      <c r="I11" s="89" t="s">
+      <c r="B11" s="91"/>
+      <c r="I11" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="89"/>
-      <c r="M11" s="93" t="s">
+      <c r="J11" s="99"/>
+      <c r="M11" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="N11" s="93"/>
-      <c r="O11" s="93"/>
-      <c r="P11" s="93"/>
+      <c r="N11" s="92"/>
+      <c r="O11" s="92"/>
+      <c r="P11" s="92"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="100"/>
+      <c r="B12" s="91"/>
       <c r="I12" s="12" t="s">
         <v>17</v>
       </c>
@@ -20096,23 +20096,23 @@
       <c r="M12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="96" t="s">
+      <c r="N12" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="O12" s="97"/>
+      <c r="O12" s="96"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="100"/>
+      <c r="B13" s="91"/>
       <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="100"/>
+      <c r="B14" s="91"/>
       <c r="I14" s="12">
         <v>125</v>
       </c>
@@ -20123,17 +20123,17 @@
       <c r="M14" s="11">
         <v>125</v>
       </c>
-      <c r="N14" s="91">
+      <c r="N14" s="101">
         <f t="shared" ref="N14:N19" si="3">(N4*surface_B2)/(1-N4)</f>
         <v>30.855561224101301</v>
       </c>
-      <c r="O14" s="92"/>
+      <c r="O14" s="102"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="100"/>
+      <c r="B15" s="91"/>
       <c r="I15" s="12">
         <v>250</v>
       </c>
@@ -20144,17 +20144,17 @@
       <c r="M15" s="11">
         <v>250</v>
       </c>
-      <c r="N15" s="91">
+      <c r="N15" s="101">
         <f t="shared" si="3"/>
         <v>47.164446345380512</v>
       </c>
-      <c r="O15" s="92"/>
+      <c r="O15" s="102"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="100"/>
+      <c r="B16" s="91"/>
       <c r="I16" s="12">
         <v>500</v>
       </c>
@@ -20165,17 +20165,17 @@
       <c r="M16" s="11">
         <v>500</v>
       </c>
-      <c r="N16" s="91">
+      <c r="N16" s="101">
         <f t="shared" si="3"/>
         <v>82.64602112870999</v>
       </c>
-      <c r="O16" s="92"/>
+      <c r="O16" s="102"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="100" t="s">
+      <c r="A17" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="100"/>
+      <c r="B17" s="91"/>
       <c r="I17" s="12">
         <v>1000</v>
       </c>
@@ -20186,11 +20186,11 @@
       <c r="M17" s="11">
         <v>1000</v>
       </c>
-      <c r="N17" s="91">
+      <c r="N17" s="101">
         <f t="shared" si="3"/>
         <v>99.987670483464015</v>
       </c>
-      <c r="O17" s="92"/>
+      <c r="O17" s="102"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I18" s="12">
@@ -20203,11 +20203,11 @@
       <c r="M18" s="11">
         <v>2000</v>
       </c>
-      <c r="N18" s="91">
+      <c r="N18" s="101">
         <f t="shared" si="3"/>
         <v>99.772538782613466</v>
       </c>
-      <c r="O18" s="92"/>
+      <c r="O18" s="102"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F19" s="13"/>
@@ -20221,25 +20221,25 @@
       <c r="M19" s="11">
         <v>4000</v>
       </c>
-      <c r="N19" s="91">
+      <c r="N19" s="101">
         <f t="shared" si="3"/>
         <v>95.013514125256648</v>
       </c>
-      <c r="O19" s="92"/>
+      <c r="O19" s="102"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C21" s="89" t="s">
+      <c r="C21" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="90"/>
-      <c r="E21" s="89" t="s">
+      <c r="D21" s="100"/>
+      <c r="E21" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="90"/>
-      <c r="I21" s="89" t="s">
+      <c r="F21" s="100"/>
+      <c r="I21" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="89"/>
+      <c r="J21" s="99"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
@@ -20387,12 +20387,15 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="N7:O7"/>
@@ -20406,15 +20409,12 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="N14:O14"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -20441,42 +20441,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="110"/>
+      <c r="B1" s="109"/>
       <c r="C1" s="24"/>
-      <c r="D1" s="113" t="s">
+      <c r="D1" s="118" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="107" t="s">
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="114" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="L1" s="107" t="s">
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="L1" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="110" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="111"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="L2" s="114"/>
-      <c r="M2" s="114"/>
-      <c r="N2" s="114"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115"/>
+      <c r="L2" s="115"/>
+      <c r="M2" s="115"/>
+      <c r="N2" s="115"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="55"/>
@@ -20494,10 +20494,10 @@
       <c r="I3" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="115" t="s">
+      <c r="J3" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="115"/>
+      <c r="K3" s="113"/>
       <c r="L3" s="44" t="s">
         <v>69</v>
       </c>
@@ -20515,17 +20515,17 @@
       <c r="B4" s="57">
         <v>58</v>
       </c>
-      <c r="C4" s="116" t="s">
+      <c r="C4" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="117"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="117"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
       <c r="G4" s="30"/>
       <c r="H4" s="27"/>
       <c r="I4" s="36"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="113"/>
       <c r="L4" s="45"/>
       <c r="M4" s="27"/>
       <c r="N4" s="30"/>
@@ -20541,10 +20541,10 @@
         <f>G5-H5</f>
         <v>60</v>
       </c>
-      <c r="J5" s="115">
+      <c r="J5" s="113">
         <v>125</v>
       </c>
-      <c r="K5" s="115"/>
+      <c r="K5" s="113"/>
       <c r="L5" s="46">
         <v>67.5</v>
       </c>
@@ -20568,10 +20568,10 @@
         <f t="shared" ref="I6:I9" si="0">G6-H6</f>
         <v>59</v>
       </c>
-      <c r="J6" s="115">
+      <c r="J6" s="113">
         <v>250</v>
       </c>
-      <c r="K6" s="115"/>
+      <c r="K6" s="113"/>
       <c r="L6" s="46">
         <v>69</v>
       </c>
@@ -20595,10 +20595,10 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="J7" s="115">
+      <c r="J7" s="113">
         <v>500</v>
       </c>
-      <c r="K7" s="115"/>
+      <c r="K7" s="113"/>
       <c r="L7" s="46">
         <v>70.5</v>
       </c>
@@ -20622,10 +20622,10 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="J8" s="115">
+      <c r="J8" s="113">
         <v>1000</v>
       </c>
-      <c r="K8" s="115"/>
+      <c r="K8" s="113"/>
       <c r="L8" s="46">
         <v>72</v>
       </c>
@@ -20662,10 +20662,10 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="J9" s="115">
+      <c r="J9" s="113">
         <v>2000</v>
       </c>
-      <c r="K9" s="115"/>
+      <c r="K9" s="113"/>
       <c r="L9" s="46">
         <v>72</v>
       </c>
@@ -20716,33 +20716,33 @@
       <c r="I12" s="40"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="106" t="s">
+      <c r="A13" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="106"/>
-      <c r="C13" s="106"/>
+      <c r="B13" s="116"/>
+      <c r="C13" s="116"/>
       <c r="F13" s="108" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="109" t="s">
+      <c r="G13" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="109" t="s">
+      <c r="H13" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="109" t="s">
+      <c r="I13" s="107" t="s">
         <v>59</v>
       </c>
       <c r="L13" s="108" t="s">
         <v>67</v>
       </c>
-      <c r="M13" s="109" t="s">
+      <c r="M13" s="107" t="s">
         <v>72</v>
       </c>
-      <c r="N13" s="109" t="s">
+      <c r="N13" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="O13" s="109" t="s">
+      <c r="O13" s="107" t="s">
         <v>59</v>
       </c>
       <c r="R13" s="31" t="s">
@@ -20754,17 +20754,17 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="106"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="106"/>
+      <c r="A14" s="116"/>
+      <c r="B14" s="116"/>
+      <c r="C14" s="116"/>
       <c r="F14" s="108"/>
-      <c r="G14" s="109"/>
-      <c r="H14" s="109"/>
-      <c r="I14" s="109"/>
+      <c r="G14" s="107"/>
+      <c r="H14" s="107"/>
+      <c r="I14" s="107"/>
       <c r="L14" s="108"/>
-      <c r="M14" s="109"/>
-      <c r="N14" s="109"/>
-      <c r="O14" s="109"/>
+      <c r="M14" s="107"/>
+      <c r="N14" s="107"/>
+      <c r="O14" s="107"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
@@ -21013,18 +21013,18 @@
         <f>IF(SUM(I17:I21) &gt; 10, "ERROR", SUM(I17:I21) )</f>
         <v>10</v>
       </c>
-      <c r="J22" s="102" t="s">
+      <c r="J22" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="K22" s="103"/>
+      <c r="K22" s="106"/>
       <c r="O22" s="50">
         <f>IF(SUM(O17:O21) &gt; 10, "ERROR", SUM(O17:O21) )</f>
         <v>8.6853992195166114</v>
       </c>
-      <c r="P22" s="102" t="s">
+      <c r="P22" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="Q22" s="103"/>
+      <c r="Q22" s="106"/>
     </row>
     <row r="24" spans="1:19" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="54"/>
@@ -21048,32 +21048,32 @@
       <c r="S24" s="54"/>
     </row>
     <row r="25" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="A25" s="110" t="s">
+      <c r="A25" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="110"/>
+      <c r="B25" s="109"/>
       <c r="C25" s="24"/>
-      <c r="D25" s="113" t="s">
+      <c r="D25" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="E25" s="113"/>
-      <c r="F25" s="113"/>
+      <c r="E25" s="118"/>
+      <c r="F25" s="118"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" s="111" t="s">
+      <c r="A26" s="110" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="111"/>
-      <c r="C26" s="111"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
+      <c r="B26" s="110"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="110"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A27" s="119" t="s">
+      <c r="A27" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="120">
+      <c r="B27" s="86">
         <v>50</v>
       </c>
       <c r="C27" s="25"/>
@@ -21084,18 +21084,18 @@
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="55"/>
       <c r="B28" s="55"/>
-      <c r="C28" s="112"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="112"/>
-      <c r="F28" s="112"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="H29" s="100" t="s">
+      <c r="H29" s="91" t="s">
         <v>93</v>
       </c>
-      <c r="I29" s="100"/>
-      <c r="J29" s="100"/>
-      <c r="K29" s="105"/>
+      <c r="I29" s="91"/>
+      <c r="J29" s="91"/>
+      <c r="K29" s="120"/>
       <c r="L29" s="28" t="s">
         <v>84</v>
       </c>
@@ -21162,38 +21162,38 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="106" t="s">
+      <c r="A34" s="116" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="106"/>
-      <c r="C34" s="106"/>
-      <c r="E34" s="107" t="s">
+      <c r="B34" s="116"/>
+      <c r="C34" s="116"/>
+      <c r="E34" s="114" t="s">
         <v>78</v>
       </c>
-      <c r="F34" s="107"/>
+      <c r="F34" s="114"/>
       <c r="H34" s="108" t="s">
         <v>67</v>
       </c>
-      <c r="I34" s="109" t="s">
+      <c r="I34" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="J34" s="109" t="s">
+      <c r="J34" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="K34" s="109" t="s">
+      <c r="K34" s="107" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="106"/>
-      <c r="B35" s="106"/>
-      <c r="C35" s="106"/>
-      <c r="E35" s="107"/>
-      <c r="F35" s="107"/>
+      <c r="A35" s="116"/>
+      <c r="B35" s="116"/>
+      <c r="C35" s="116"/>
+      <c r="E35" s="114"/>
+      <c r="F35" s="114"/>
       <c r="H35" s="108"/>
-      <c r="I35" s="109"/>
-      <c r="J35" s="109"/>
-      <c r="K35" s="109"/>
+      <c r="I35" s="107"/>
+      <c r="J35" s="107"/>
+      <c r="K35" s="107"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
@@ -21331,11 +21331,11 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="L40" s="104" t="s">
+      <c r="L40" s="119" t="s">
         <v>83</v>
       </c>
-      <c r="M40" s="100"/>
-      <c r="N40" s="100"/>
+      <c r="M40" s="91"/>
+      <c r="N40" s="91"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
@@ -21417,13 +21417,37 @@
         <f>IF(SUM(K38:K42) &gt; 10, "ERROR", SUM(K38:K42) )</f>
         <v>8.8282406190027132</v>
       </c>
-      <c r="L43" s="102" t="s">
+      <c r="L43" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="M43" s="103"/>
+      <c r="M43" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="A34:C35"/>
+    <mergeCell ref="E34:F35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="L1:N2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="F13:F14"/>
@@ -21437,30 +21461,6 @@
     <mergeCell ref="G1:I2"/>
     <mergeCell ref="A13:C14"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="L1:N2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="A34:C35"/>
-    <mergeCell ref="E34:F35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="K34:K35"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21487,17 +21487,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="H1" s="118" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="H1" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
       <c r="K1" s="69" t="s">
         <v>101</v>
       </c>

</xml_diff>